<commit_message>
add no assembly flow
</commit_message>
<xml_diff>
--- a/pbgi_configuration_template.xlsx
+++ b/pbgi_configuration_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E16E81D-08D7-4442-9E32-B5A82CE44B1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909ECA81-EC78-4D39-A667-769ADCFF2BFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="200">
   <si>
     <t>enable</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -655,6 +655,10 @@
   </si>
   <si>
     <t>minOverlapLength=</t>
+  </si>
+  <si>
+    <t>assembly_enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2074,7 +2078,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2128,8 +2132,12 @@
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="2" t="b">
+        <v>1</v>
+      </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="10"/>

</xml_diff>